<commit_message>
upload new dataset and general update
</commit_message>
<xml_diff>
--- a/data/DS_Visualizer_Features.xlsx
+++ b/data/DS_Visualizer_Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Altri computer\Computer_Laboratorio\AntonioM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Il mio Drive\Prediction_Flavoprotein_EM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92625442-2C82-421E-A655-4E9B491270CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AA3A52-5138-435E-99EF-4862B1AF152D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,6 @@
     <t>PDB ID</t>
   </si>
   <si>
-    <t>Pymol_N1-N3</t>
-  </si>
-  <si>
-    <t>Pymol_O</t>
-  </si>
-  <si>
-    <t>Pymol_Pi-Pistacking</t>
-  </si>
-  <si>
-    <t>Pymol_Stackingalifatico</t>
-  </si>
-  <si>
-    <t>Pymol_Pi Cation</t>
-  </si>
-  <si>
     <t>1AG9</t>
   </si>
   <si>
@@ -524,6 +509,21 @@
   </si>
   <si>
     <t>3GYJ</t>
+  </si>
+  <si>
+    <t>N1-N3 _Hbond</t>
+  </si>
+  <si>
+    <t>O _Hbond</t>
+  </si>
+  <si>
+    <t>Pi-Pi_Stacking</t>
+  </si>
+  <si>
+    <t>Pi_Cation</t>
+  </si>
+  <si>
+    <t>Stacking_Alifatico</t>
   </si>
 </sst>
 </file>
@@ -582,13 +582,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,19 +934,19 @@
   <dimension ref="A1:G164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J157" sqref="J157"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G152" sqref="G152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22" style="2" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
@@ -952,19 +955,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>164</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>165</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -972,7 +975,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -995,7 +998,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -1018,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -1041,7 +1044,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
@@ -1064,7 +1067,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -1087,7 +1090,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -1110,7 +1113,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
@@ -1133,7 +1136,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -1156,7 +1159,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -1179,7 +1182,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -1202,7 +1205,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -1225,7 +1228,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -1248,7 +1251,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
@@ -1271,7 +1274,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
@@ -1294,7 +1297,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2">
         <v>0</v>
@@ -1317,7 +1320,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2">
         <v>2</v>
@@ -1340,7 +1343,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
@@ -1363,7 +1366,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
@@ -1386,7 +1389,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C20" s="2">
         <v>2</v>
@@ -1409,7 +1412,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2">
         <v>2</v>
@@ -1432,7 +1435,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C22" s="2">
         <v>2</v>
@@ -1455,7 +1458,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2">
         <v>2</v>
@@ -1478,7 +1481,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C24" s="2">
         <v>1</v>
@@ -1501,7 +1504,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C25" s="2">
         <v>2</v>
@@ -1524,7 +1527,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2">
         <v>2</v>
@@ -1547,7 +1550,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
@@ -1570,7 +1573,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C28" s="2">
         <v>2</v>
@@ -1593,7 +1596,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
@@ -1616,7 +1619,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C30" s="2">
         <v>2</v>
@@ -1639,7 +1642,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C31" s="2">
         <v>2</v>
@@ -1662,7 +1665,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
@@ -1685,7 +1688,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
@@ -1708,7 +1711,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
@@ -1731,7 +1734,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C35" s="2">
         <v>2</v>
@@ -1754,7 +1757,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C36" s="2">
         <v>1</v>
@@ -1777,7 +1780,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C37" s="2">
         <v>0</v>
@@ -1800,7 +1803,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C38" s="2">
         <v>2</v>
@@ -1823,7 +1826,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C39" s="2">
         <v>2</v>
@@ -1846,7 +1849,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C40" s="2">
         <v>2</v>
@@ -1869,7 +1872,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C41" s="2">
         <v>2</v>
@@ -1892,7 +1895,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C42" s="2">
         <v>2</v>
@@ -1915,7 +1918,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -1938,7 +1941,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C44" s="2">
         <v>2</v>
@@ -1961,7 +1964,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C45" s="2">
         <v>0</v>
@@ -1984,7 +1987,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C46" s="2">
         <v>1</v>
@@ -2007,7 +2010,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C47" s="2">
         <v>2</v>
@@ -2030,7 +2033,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C48" s="2">
         <v>1</v>
@@ -2053,7 +2056,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C49" s="2">
         <v>1</v>
@@ -2076,7 +2079,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C50" s="2">
         <v>1</v>
@@ -2099,7 +2102,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C51" s="2">
         <v>1</v>
@@ -2122,7 +2125,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C52" s="2">
         <v>1</v>
@@ -2145,7 +2148,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C53" s="2">
         <v>1</v>
@@ -2168,7 +2171,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C54" s="2">
         <v>2</v>
@@ -2191,7 +2194,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C55" s="2">
         <v>1</v>
@@ -2214,7 +2217,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C56" s="2">
         <v>2</v>
@@ -2237,7 +2240,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C57" s="2">
         <v>1</v>
@@ -2260,7 +2263,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C58" s="2">
         <v>0</v>
@@ -2283,7 +2286,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C59" s="2">
         <v>2</v>
@@ -2306,7 +2309,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C60" s="2">
         <v>2</v>
@@ -2329,7 +2332,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C61" s="2">
         <v>1</v>
@@ -2352,7 +2355,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C62" s="2">
         <v>1</v>
@@ -2375,7 +2378,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C63" s="2">
         <v>0</v>
@@ -2398,7 +2401,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C64" s="2">
         <v>2</v>
@@ -2421,7 +2424,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C65" s="2">
         <v>1</v>
@@ -2444,7 +2447,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C66" s="2">
         <v>1</v>
@@ -2467,7 +2470,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C67" s="2">
         <v>1</v>
@@ -2490,7 +2493,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C68" s="2">
         <v>1</v>
@@ -2513,7 +2516,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C69" s="2">
         <v>1</v>
@@ -2536,7 +2539,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C70" s="2">
         <v>1</v>
@@ -2559,7 +2562,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C71" s="2">
         <v>1</v>
@@ -2582,7 +2585,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C72" s="2">
         <v>1</v>
@@ -2605,7 +2608,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C73" s="2">
         <v>2</v>
@@ -2628,7 +2631,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C74" s="2">
         <v>2</v>
@@ -2651,7 +2654,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C75" s="2">
         <v>2</v>
@@ -2674,7 +2677,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C76" s="2">
         <v>2</v>
@@ -2697,7 +2700,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C77" s="2">
         <v>2</v>
@@ -2720,7 +2723,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C78" s="2">
         <v>1</v>
@@ -2743,7 +2746,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C79" s="2">
         <v>1</v>
@@ -2766,7 +2769,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C80" s="2">
         <v>3</v>
@@ -2789,7 +2792,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C81" s="2">
         <v>2</v>
@@ -2812,7 +2815,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C82" s="2">
         <v>1</v>
@@ -2835,7 +2838,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C83" s="2">
         <v>0</v>
@@ -2858,7 +2861,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C84" s="2">
         <v>1</v>
@@ -2881,7 +2884,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C85" s="2">
         <v>1</v>
@@ -2904,7 +2907,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C86" s="2">
         <v>1</v>
@@ -2927,7 +2930,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C87" s="2">
         <v>2</v>
@@ -2950,7 +2953,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C88" s="2">
         <v>1</v>
@@ -2973,7 +2976,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C89" s="2">
         <v>1</v>
@@ -2996,7 +2999,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C90" s="2">
         <v>1</v>
@@ -3019,7 +3022,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C91" s="2">
         <v>1</v>
@@ -3042,7 +3045,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C92" s="2">
         <v>1</v>
@@ -3065,7 +3068,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C93" s="2">
         <v>2</v>
@@ -3088,7 +3091,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C94" s="2">
         <v>1</v>
@@ -3111,7 +3114,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C95" s="2">
         <v>1</v>
@@ -3134,7 +3137,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C96" s="2">
         <v>1</v>
@@ -3157,7 +3160,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C97" s="2">
         <v>1</v>
@@ -3180,7 +3183,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C98" s="2">
         <v>2</v>
@@ -3203,7 +3206,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C99" s="2">
         <v>1</v>
@@ -3226,7 +3229,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C100" s="2">
         <v>2</v>
@@ -3249,7 +3252,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C101" s="2">
         <v>2</v>
@@ -3272,7 +3275,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C102" s="2">
         <v>3</v>
@@ -3295,7 +3298,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C103" s="2">
         <v>0</v>
@@ -3318,7 +3321,7 @@
         <v>102</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C104" s="2">
         <v>0</v>
@@ -3341,7 +3344,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C105" s="2">
         <v>1</v>
@@ -3364,7 +3367,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C106" s="2">
         <v>3</v>
@@ -3387,7 +3390,7 @@
         <v>105</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C107" s="2">
         <v>2</v>
@@ -3410,7 +3413,7 @@
         <v>106</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C108" s="2">
         <v>2</v>
@@ -3433,7 +3436,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C109" s="2">
         <v>1</v>
@@ -3456,7 +3459,7 @@
         <v>108</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C110" s="2">
         <v>2</v>
@@ -3479,7 +3482,7 @@
         <v>109</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C111" s="2">
         <v>1</v>
@@ -3502,7 +3505,7 @@
         <v>110</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C112" s="2">
         <v>1</v>
@@ -3525,7 +3528,7 @@
         <v>111</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C113" s="2">
         <v>1</v>
@@ -3548,7 +3551,7 @@
         <v>112</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C114" s="2">
         <v>2</v>
@@ -3571,7 +3574,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C115" s="2">
         <v>2</v>
@@ -3594,7 +3597,7 @@
         <v>114</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C116" s="2">
         <v>2</v>
@@ -3617,7 +3620,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C117" s="2">
         <v>2</v>
@@ -3640,7 +3643,7 @@
         <v>116</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C118" s="2">
         <v>1</v>
@@ -3663,7 +3666,7 @@
         <v>117</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C119" s="2">
         <v>2</v>
@@ -3686,7 +3689,7 @@
         <v>118</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C120" s="2">
         <v>2</v>
@@ -3709,7 +3712,7 @@
         <v>119</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C121" s="2">
         <v>2</v>
@@ -3732,7 +3735,7 @@
         <v>120</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C122" s="2">
         <v>1</v>
@@ -3755,7 +3758,7 @@
         <v>121</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C123" s="2">
         <v>2</v>
@@ -3778,7 +3781,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C124" s="2">
         <v>0</v>
@@ -3801,7 +3804,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C125" s="2">
         <v>1</v>
@@ -3824,7 +3827,7 @@
         <v>124</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C126" s="2">
         <v>1</v>
@@ -3847,7 +3850,7 @@
         <v>125</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C127" s="2">
         <v>2</v>
@@ -3870,7 +3873,7 @@
         <v>126</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C128" s="2">
         <v>1</v>
@@ -3893,7 +3896,7 @@
         <v>127</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C129" s="2">
         <v>1</v>
@@ -3916,7 +3919,7 @@
         <v>128</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C130" s="2">
         <v>1</v>
@@ -3939,7 +3942,7 @@
         <v>129</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C131" s="2">
         <v>2</v>
@@ -3962,7 +3965,7 @@
         <v>130</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C132" s="2">
         <v>2</v>
@@ -3985,7 +3988,7 @@
         <v>131</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C133" s="2">
         <v>2</v>
@@ -4008,7 +4011,7 @@
         <v>132</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C134" s="2">
         <v>2</v>
@@ -4031,7 +4034,7 @@
         <v>133</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C135" s="2">
         <v>2</v>
@@ -4054,7 +4057,7 @@
         <v>134</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C136" s="2">
         <v>2</v>
@@ -4077,7 +4080,7 @@
         <v>135</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C137" s="2">
         <v>2</v>
@@ -4100,7 +4103,7 @@
         <v>136</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C138" s="2">
         <v>1</v>
@@ -4123,7 +4126,7 @@
         <v>137</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C139" s="2">
         <v>1</v>
@@ -4146,7 +4149,7 @@
         <v>138</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C140" s="2">
         <v>1</v>
@@ -4169,7 +4172,7 @@
         <v>139</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C141" s="2">
         <v>2</v>
@@ -4192,7 +4195,7 @@
         <v>140</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C142" s="2">
         <v>1</v>
@@ -4215,7 +4218,7 @@
         <v>141</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C143" s="2">
         <v>1</v>
@@ -4238,7 +4241,7 @@
         <v>142</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C144" s="2">
         <v>2</v>
@@ -4261,7 +4264,7 @@
         <v>143</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C145" s="2">
         <v>0</v>
@@ -4284,7 +4287,7 @@
         <v>144</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C146" s="2">
         <v>2</v>
@@ -4307,7 +4310,7 @@
         <v>145</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C147" s="2">
         <v>2</v>
@@ -4330,7 +4333,7 @@
         <v>146</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C148" s="2">
         <v>1</v>
@@ -4353,7 +4356,7 @@
         <v>147</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C149" s="2">
         <v>2</v>
@@ -4376,7 +4379,7 @@
         <v>148</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C150" s="2">
         <v>2</v>
@@ -4399,7 +4402,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C151" s="2">
         <v>1</v>
@@ -4422,7 +4425,7 @@
         <v>150</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C152" s="2">
         <v>1</v>
@@ -4445,7 +4448,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C153" s="2">
         <v>1</v>
@@ -4468,7 +4471,7 @@
         <v>152</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C154" s="2">
         <v>1</v>
@@ -4491,7 +4494,7 @@
         <v>153</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C155" s="2">
         <v>2</v>
@@ -4514,7 +4517,7 @@
         <v>154</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C156" s="2">
         <v>1</v>
@@ -4537,7 +4540,7 @@
         <v>155</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C157" s="2">
         <v>2</v>
@@ -4560,7 +4563,7 @@
         <v>156</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C158" s="2">
         <v>1</v>
@@ -4583,7 +4586,7 @@
         <v>157</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C159" s="2">
         <v>2</v>
@@ -4606,7 +4609,7 @@
         <v>158</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C160" s="2">
         <v>1</v>
@@ -4629,7 +4632,7 @@
         <v>159</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C161" s="2">
         <v>1</v>
@@ -4652,7 +4655,7 @@
         <v>160</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C162" s="2">
         <v>2</v>
@@ -4675,7 +4678,7 @@
         <v>161</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C163" s="2">
         <v>2</v>
@@ -4698,7 +4701,7 @@
         <v>162</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C164" s="2">
         <v>2</v>

</xml_diff>